<commit_message>
Changes in whole structure
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Xpaths.xlsx
+++ b/src/test/resources/TestData/Xpaths.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10711204\eclipse-workspace\Automation_UI\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10711204\Desktop\First push\ABDM_Automatrion_Framework\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0128DD49-B248-42F3-A5E3-DC85A0E5C685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7789D2C-67D4-4A61-9107-E6016042D167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -468,7 +468,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>